<commit_message>
Updated convert_excel_date to throw ValueError when input- column values are of type non-numeric
</commit_message>
<xml_diff>
--- a/examples/notebooks/dirty_data.xlsx
+++ b/examples/notebooks/dirty_data.xlsx
@@ -1,35 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFirke\Documents\Bitbucket\janitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.nimmagadda\Desktop\Learning\github-projects\pyjanitor\examples\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E15B1F-1CF6-4871-97B9-2B9DE146C5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6072"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam Firke</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>Teacher</t>
   </si>
@@ -211,12 +220,21 @@
   </si>
   <si>
     <t>Basketball</t>
+  </si>
+  <si>
+    <t>Hire Date Str</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>maths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -313,10 +331,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,28 +647,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.05078125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -685,8 +701,11 @@
       <c r="K1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -699,7 +718,7 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>39690</v>
       </c>
       <c r="F2" s="2">
@@ -715,9 +734,11 @@
       <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2" s="12">
+        <v>39690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -730,7 +751,7 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>39690</v>
       </c>
       <c r="F3" s="2">
@@ -746,9 +767,11 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L3" s="10">
+        <v>39690</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -761,7 +784,7 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>37118</v>
       </c>
       <c r="F4" s="2">
@@ -777,9 +800,11 @@
       <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L4" s="10">
+        <v>37118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -793,7 +818,7 @@
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>27515</v>
       </c>
       <c r="F5" s="2">
@@ -809,9 +834,11 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L5" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -824,7 +851,7 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>41431</v>
       </c>
       <c r="F6" s="2">
@@ -837,9 +864,11 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L6" s="10">
+        <v>41431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -852,7 +881,7 @@
       <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>11037</v>
       </c>
       <c r="F7" s="2">
@@ -868,9 +897,11 @@
       <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L7" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -883,7 +914,7 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>11037</v>
       </c>
       <c r="F8" s="2">
@@ -899,13 +930,15 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="13"/>
+      <c r="L8" s="10">
+        <v>11037</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -918,7 +951,7 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>32994</v>
       </c>
       <c r="F10" s="2">
@@ -931,9 +964,11 @@
       <c r="J10" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L10" s="10">
+        <v>32994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -946,7 +981,7 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>27919</v>
       </c>
       <c r="F11" s="2">
@@ -959,9 +994,11 @@
       <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L11" s="10">
+        <v>27919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -974,7 +1011,7 @@
       <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>42221</v>
       </c>
       <c r="F12" t="e">
@@ -988,9 +1025,11 @@
       <c r="I12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="10">
+        <v>42221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1000,7 +1039,7 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>34700</v>
       </c>
       <c r="F13" t="e">
@@ -1014,9 +1053,11 @@
       <c r="J13" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="10">
+        <v>34700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1070,7 @@
       <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>40071</v>
       </c>
       <c r="F14" s="2">
@@ -1045,18 +1086,20 @@
       <c r="J14" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="10">
+        <v>40071</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H18" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ENH] Updated convert_excel_date to throw meaningful error (#841)
* Updated convert_excel_date to throw ValueError when input- column values are of type non-numeric

* Updated Changelog

* Fixed Code formatting and linting issues

* Notebook converting_currency Error Fix
</commit_message>
<xml_diff>
--- a/examples/notebooks/dirty_data.xlsx
+++ b/examples/notebooks/dirty_data.xlsx
@@ -1,35 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFirke\Documents\Bitbucket\janitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.nimmagadda\Desktop\Learning\github-projects\pyjanitor\examples\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E15B1F-1CF6-4871-97B9-2B9DE146C5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6072"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam Firke</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>Teacher</t>
   </si>
@@ -211,12 +220,21 @@
   </si>
   <si>
     <t>Basketball</t>
+  </si>
+  <si>
+    <t>Hire Date Str</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>maths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -313,10 +331,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,28 +647,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.05078125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -685,8 +701,11 @@
       <c r="K1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -699,7 +718,7 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>39690</v>
       </c>
       <c r="F2" s="2">
@@ -715,9 +734,11 @@
       <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L2" s="12">
+        <v>39690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -730,7 +751,7 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>39690</v>
       </c>
       <c r="F3" s="2">
@@ -746,9 +767,11 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L3" s="10">
+        <v>39690</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -761,7 +784,7 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>37118</v>
       </c>
       <c r="F4" s="2">
@@ -777,9 +800,11 @@
       <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L4" s="10">
+        <v>37118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -793,7 +818,7 @@
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>27515</v>
       </c>
       <c r="F5" s="2">
@@ -809,9 +834,11 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L5" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -824,7 +851,7 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>41431</v>
       </c>
       <c r="F6" s="2">
@@ -837,9 +864,11 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L6" s="10">
+        <v>41431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -852,7 +881,7 @@
       <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>11037</v>
       </c>
       <c r="F7" s="2">
@@ -868,9 +897,11 @@
       <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L7" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -883,7 +914,7 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>11037</v>
       </c>
       <c r="F8" s="2">
@@ -899,13 +930,15 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="13"/>
+      <c r="L8" s="10">
+        <v>11037</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -918,7 +951,7 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>32994</v>
       </c>
       <c r="F10" s="2">
@@ -931,9 +964,11 @@
       <c r="J10" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L10" s="10">
+        <v>32994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -946,7 +981,7 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>27919</v>
       </c>
       <c r="F11" s="2">
@@ -959,9 +994,11 @@
       <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L11" s="10">
+        <v>27919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -974,7 +1011,7 @@
       <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>42221</v>
       </c>
       <c r="F12" t="e">
@@ -988,9 +1025,11 @@
       <c r="I12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="10">
+        <v>42221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1000,7 +1039,7 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>34700</v>
       </c>
       <c r="F13" t="e">
@@ -1014,9 +1053,11 @@
       <c r="J13" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="10">
+        <v>34700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1070,7 @@
       <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>40071</v>
       </c>
       <c r="F14" s="2">
@@ -1045,18 +1086,20 @@
       <c r="J14" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="10">
+        <v>40071</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H18" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DOC]Add missing functions to API docs Index (#872)
* add factorize_columns and drop_constant_columns to the API index

* fix spelling in changelog

* delete pytest.ini and update pyproject.toml
</commit_message>
<xml_diff>
--- a/examples/notebooks/dirty_data.xlsx
+++ b/examples/notebooks/dirty_data.xlsx
@@ -1,44 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.nimmagadda\Desktop\Learning\github-projects\pyjanitor\examples\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFirke\Documents\Bitbucket\janitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E15B1F-1CF6-4871-97B9-2B9DE146C5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam Firke</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Teacher</t>
   </si>
@@ -220,21 +211,12 @@
   </si>
   <si>
     <t>Basketball</t>
-  </si>
-  <si>
-    <t>Hire Date Str</t>
-  </si>
-  <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>maths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -331,9 +313,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,27 +630,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.62890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.05078125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -701,11 +685,8 @@
       <c r="K1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -718,7 +699,7 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="12">
         <v>39690</v>
       </c>
       <c r="F2" s="2">
@@ -734,11 +715,9 @@
       <c r="J2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="12">
-        <v>39690</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -751,7 +730,7 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="12">
         <v>39690</v>
       </c>
       <c r="F3" s="2">
@@ -767,11 +746,9 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="10">
-        <v>39690</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -784,7 +761,7 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="12">
         <v>37118</v>
       </c>
       <c r="F4" s="2">
@@ -800,11 +777,9 @@
       <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="10">
-        <v>37118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -818,7 +793,7 @@
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>27515</v>
       </c>
       <c r="F5" s="2">
@@ -834,11 +809,9 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -851,7 +824,7 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="12">
         <v>41431</v>
       </c>
       <c r="F6" s="2">
@@ -864,11 +837,9 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="10">
-        <v>41431</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -881,7 +852,7 @@
       <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="12">
         <v>11037</v>
       </c>
       <c r="F7" s="2">
@@ -897,11 +868,9 @@
       <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -914,7 +883,7 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="12">
         <v>11037</v>
       </c>
       <c r="F8" s="2">
@@ -930,15 +899,13 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="10">
-        <v>11037</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="11"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="13"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -951,7 +918,7 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="12">
         <v>32994</v>
       </c>
       <c r="F10" s="2">
@@ -964,11 +931,9 @@
       <c r="J10" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="10">
-        <v>32994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -981,7 +946,7 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="12">
         <v>27919</v>
       </c>
       <c r="F11" s="2">
@@ -994,11 +959,9 @@
       <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="10">
-        <v>27919</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +974,7 @@
       <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="12">
         <v>42221</v>
       </c>
       <c r="F12" t="e">
@@ -1025,11 +988,9 @@
       <c r="I12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="10">
-        <v>42221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1000,7 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="12">
         <v>34700</v>
       </c>
       <c r="F13" t="e">
@@ -1053,11 +1014,9 @@
       <c r="J13" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="10">
-        <v>34700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1029,7 @@
       <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="12">
         <v>40071</v>
       </c>
       <c r="F14" s="2">
@@ -1086,20 +1045,18 @@
       <c r="J14" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="10">
-        <v>40071</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H18" s="1"/>
     </row>
   </sheetData>

</xml_diff>